<commit_message>
Adds new test stembureau spreadsheet
</commit_message>
<xml_diff>
--- a/tests/data/waarismijnstemlokaal.nl_invulformulier.xlsx
+++ b/tests/data/waarismijnstemlokaal.nl_invulformulier.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Toelichting" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Attributen" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Metadata" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Toelichting" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Attributen" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Metadata" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="1160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="1162">
   <si>
     <t xml:space="preserve">Toelichting</t>
   </si>
@@ -3191,7 +3191,10 @@
     <t xml:space="preserve">2024-06-06T07:30:00</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-06-06T02:30:00</t>
+    <t xml:space="preserve">2025-10-29T07:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-10-29T02:30:00</t>
   </si>
   <si>
     <t xml:space="preserve">Sluitingstijd</t>
@@ -3200,7 +3203,10 @@
     <t xml:space="preserve">2024-06-06T21:00:00</t>
   </si>
   <si>
-    <t xml:space="preserve">2024-06-06T20:00:00</t>
+    <t xml:space="preserve">2025-10-29T21:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-10-29T20:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">Toegankelijk voor mensen met een lichamelijke beperking</t>
@@ -4021,39 +4027,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4065,19 +4071,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4085,11 +4091,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4109,15 +4115,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4129,15 +4135,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4153,15 +4159,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4177,11 +4183,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4189,7 +4195,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4197,7 +4203,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4205,7 +4211,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="59" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4225,7 +4231,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4346,18 +4352,124 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="78.19"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="2" width="10.82"/>
@@ -4370,7 +4482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4380,7 +4492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="180.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -4413,18 +4525,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:AMJ30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="G28" activeCellId="0" sqref="G28"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="51.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7667,7 +7779,7 @@
       <c r="AMI5" s="6"/>
       <c r="AMJ5" s="6"/>
     </row>
-    <row r="6" s="9" customFormat="true" ht="202.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="9" customFormat="true" ht="225.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
         <v>1027</v>
       </c>
@@ -7720,7 +7832,7 @@
       <c r="AMI6" s="6"/>
       <c r="AMJ6" s="6"/>
     </row>
-    <row r="7" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="9" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
         <v>1030</v>
       </c>
@@ -7771,7 +7883,7 @@
       <c r="AMI7" s="6"/>
       <c r="AMJ7" s="6"/>
     </row>
-    <row r="8" s="9" customFormat="true" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="9" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
         <v>1035</v>
       </c>
@@ -7824,7 +7936,7 @@
       <c r="AMI8" s="6"/>
       <c r="AMJ8" s="6"/>
     </row>
-    <row r="9" s="9" customFormat="true" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="9" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
         <v>1039</v>
       </c>
@@ -7877,7 +7989,7 @@
       <c r="AMI9" s="6"/>
       <c r="AMJ9" s="6"/>
     </row>
-    <row r="10" s="9" customFormat="true" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" s="9" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
         <v>1042</v>
       </c>
@@ -7930,7 +8042,7 @@
       <c r="AMI10" s="6"/>
       <c r="AMJ10" s="6"/>
     </row>
-    <row r="11" s="9" customFormat="true" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="9" customFormat="true" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
         <v>1045</v>
       </c>
@@ -7983,7 +8095,7 @@
       <c r="AMI11" s="6"/>
       <c r="AMJ11" s="6"/>
     </row>
-    <row r="12" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="24" t="s">
         <v>1047</v>
       </c>
@@ -8000,10 +8112,10 @@
         <v>1050</v>
       </c>
       <c r="F12" s="26" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -8036,9 +8148,9 @@
       <c r="AMI12" s="6"/>
       <c r="AMJ12" s="6"/>
     </row>
-    <row r="13" s="9" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="24" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>1011</v>
@@ -8050,13 +8162,13 @@
         <v>1049</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="G13" s="26" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
@@ -8091,16 +8203,16 @@
     </row>
     <row r="14" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>1011</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>1011</v>
@@ -8144,16 +8256,16 @@
     </row>
     <row r="15" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C15" s="15" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>1059</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>1057</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>1011</v>
@@ -8197,16 +8309,16 @@
     </row>
     <row r="16" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>1011</v>
@@ -8250,16 +8362,16 @@
     </row>
     <row r="17" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>1011</v>
@@ -8303,22 +8415,22 @@
     </row>
     <row r="18" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="G18" s="19" t="s">
         <v>1023</v>
@@ -8354,18 +8466,18 @@
       <c r="AMI18" s="6"/>
       <c r="AMJ18" s="6"/>
     </row>
-    <row r="19" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" s="9" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>1011</v>
@@ -8409,16 +8521,16 @@
     </row>
     <row r="20" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>1011</v>
@@ -8462,16 +8574,16 @@
     </row>
     <row r="21" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>1011</v>
@@ -8513,24 +8625,24 @@
       <c r="AMI21" s="6"/>
       <c r="AMJ21" s="6"/>
     </row>
-    <row r="22" s="9" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" s="9" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>1023</v>
@@ -8568,16 +8680,16 @@
     </row>
     <row r="23" s="9" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>1011</v>
@@ -8619,18 +8731,18 @@
       <c r="AMI23" s="6"/>
       <c r="AMJ23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E24" s="19" t="s">
         <v>1011</v>
@@ -8644,16 +8756,16 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>1011</v>
@@ -8665,36 +8777,36 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="G26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>1033</v>
@@ -8705,16 +8817,16 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>1023</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E28" s="27" t="s">
         <v>1011</v>
@@ -8728,48 +8840,48 @@
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="28" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>1011</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="F29" s="29" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="28" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>1011</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>1025</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="F30" s="29" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
     </row>
   </sheetData>
@@ -8784,7 +8896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -8831,19 +8943,19 @@
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="37" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>1011</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
@@ -8861,37 +8973,37 @@
     </row>
     <row r="3" s="6" customFormat="true" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="40" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>1023</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>1105</v>
+        <v>1107</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="41" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>1011</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
@@ -8909,19 +9021,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="41" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="B5" s="43" t="s">
         <v>1011</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D5" s="45" t="s">
         <v>1015</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="34"/>
@@ -8939,19 +9051,19 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="41" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="B6" s="43" t="s">
         <v>1011</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D6" s="46" t="s">
         <v>1015</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
@@ -8967,21 +9079,21 @@
       <c r="Q6" s="34"/>
       <c r="R6" s="34"/>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="B7" s="43" t="s">
         <v>1023</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D7" s="46" t="s">
         <v>1015</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="F7" s="34"/>
       <c r="G7" s="34"/>
@@ -8999,19 +9111,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="41" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="B8" s="43" t="s">
         <v>1023</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D8" s="46" t="s">
         <v>1015</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
@@ -9027,21 +9139,21 @@
       <c r="Q8" s="34"/>
       <c r="R8" s="34"/>
     </row>
-    <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="41" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>1023</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="34"/>
@@ -9059,17 +9171,17 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="41" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="B10" s="43" t="s">
         <v>1011</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D10" s="46"/>
       <c r="E10" s="46" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="34"/>
@@ -9087,17 +9199,17 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="41" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="B11" s="43" t="s">
         <v>1011</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D11" s="46"/>
       <c r="E11" s="46" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="F11" s="39"/>
       <c r="G11" s="34"/>
@@ -9115,19 +9227,19 @@
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>1023</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="34"/>
@@ -9145,19 +9257,19 @@
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
       <c r="B13" s="36" t="s">
         <v>1011</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="E13" s="47" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
@@ -9175,17 +9287,17 @@
     </row>
     <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="B14" s="43" t="s">
         <v>1023</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D14" s="48"/>
       <c r="E14" s="48" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="18"/>
@@ -9203,19 +9315,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>1023</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="18"/>
@@ -9233,19 +9345,19 @@
     </row>
     <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="41" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="B16" s="36" t="s">
         <v>1011</v>
       </c>
       <c r="C16" s="35" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="D16" s="50" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="E16" s="50" t="s">
-        <v>1145</v>
+        <v>1147</v>
       </c>
       <c r="F16" s="34"/>
       <c r="G16" s="34"/>
@@ -9263,19 +9375,19 @@
     </row>
     <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>1146</v>
+        <v>1148</v>
       </c>
       <c r="B17" s="36" t="s">
         <v>1011</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="E17" s="47" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="34"/>
@@ -9293,17 +9405,17 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41" t="s">
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="B18" s="43" t="s">
         <v>1011</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D18" s="51"/>
       <c r="E18" s="51" t="s">
-        <v>1149</v>
+        <v>1151</v>
       </c>
       <c r="F18" s="39"/>
       <c r="G18" s="34"/>
@@ -9321,17 +9433,17 @@
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="41" t="s">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="B19" s="43" t="s">
         <v>1023</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>1151</v>
+        <v>1153</v>
       </c>
       <c r="D19" s="48"/>
       <c r="E19" s="45" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="18"/>
@@ -9349,19 +9461,19 @@
     </row>
     <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
       <c r="B20" s="36" t="s">
         <v>1023</v>
       </c>
       <c r="C20" s="35" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="D20" s="42" t="s">
-        <v>1155</v>
+        <v>1157</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>1156</v>
+        <v>1158</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="34"/>
@@ -9379,16 +9491,16 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="40" t="s">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>1011</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>1158</v>
+        <v>1160</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>1159</v>
+        <v>1161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>